<commit_message>
modify line height for fig descriptions
</commit_message>
<xml_diff>
--- a/docs/figureinfo/TOGS-lof5.xlsx
+++ b/docs/figureinfo/TOGS-lof5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R\Rprojects\HistDataVis\figureinfo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2DDD0F9-9F7F-45E1-9B74-D76906499C54}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5277208-0F4F-4CD2-B3D2-517B1F37A426}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="285" yWindow="585" windowWidth="24285" windowHeight="13890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1540,9 +1540,6 @@
     <t xml:space="preserve">Farr’s radial diagram of temperature and mortality in London by week for the years 1840–1850. The yearly charts are arranged row-wise from 1840 at the top left. The chart at the bottom right corner shows the average over the years 1840–1849. In each chart, weeks of the year are arranged clockwise, starting from January 1 at 6:35. </t>
   </si>
   <si>
-    <t xml:space="preserve">Re-drawn and enhanced versions of a central portion of Snow’s map of the cholera data using the most historically accurate known data digitized from the map. Deaths are shown by the jittered points, and the six pumps in this region by labeled triangles. Two guides for interpretation were added: Voronoi polygons showing the region of the map closest to each pump (left), and shaded contours of the intensity of deaths from cholera (right). </t>
-  </si>
-  <si>
     <t xml:space="preserve">A radial diagram showing the number of deaths from preventible zymotic diseases (outer, blue wedges) compared with deaths from wounds (red) and from all other causes (gray). Right: data for April 1854 to March 1855; left: data for April 1855 to March 1865 after the arrival of the Sanitary Commission. </t>
   </si>
   <si>
@@ -1895,6 +1892,9 @@
   </si>
   <si>
     <t>Time line of milestone events</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Re-drawn and enhanced versions of a central portion of Snow’s map of the cholera data using the most historically accurate known data digitized from the map. Deaths are shown by the jittered points, and the six pumps in this region by labeled triangles. Two guides for interpretation were added: Voronoi polygons showing the region of the map closest to each pump (top), and shaded contours of the intensity of deaths from cholera (bottom). </t>
   </si>
 </sst>
 </file>
@@ -2249,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2297,13 +2297,13 @@
         <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F2" t="s">
         <v>394</v>
       </c>
       <c r="G2" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2323,10 +2323,10 @@
         <v>266</v>
       </c>
       <c r="F3" t="s">
+        <v>621</v>
+      </c>
+      <c r="G3" t="s">
         <v>622</v>
-      </c>
-      <c r="G3" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2349,7 +2349,7 @@
         <v>395</v>
       </c>
       <c r="G4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2372,7 +2372,7 @@
         <v>396</v>
       </c>
       <c r="G5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
         <v>397</v>
       </c>
       <c r="G6" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2418,7 +2418,7 @@
         <v>398</v>
       </c>
       <c r="G7" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2441,7 +2441,7 @@
         <v>399</v>
       </c>
       <c r="G8" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2464,7 +2464,7 @@
         <v>400</v>
       </c>
       <c r="G9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2487,7 +2487,7 @@
         <v>401</v>
       </c>
       <c r="G10" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -2510,7 +2510,7 @@
         <v>402</v>
       </c>
       <c r="G11" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -2533,7 +2533,7 @@
         <v>403</v>
       </c>
       <c r="G12" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -2556,7 +2556,7 @@
         <v>404</v>
       </c>
       <c r="G13" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2579,7 +2579,7 @@
         <v>405</v>
       </c>
       <c r="G14" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -2602,7 +2602,7 @@
         <v>406</v>
       </c>
       <c r="G15" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -2625,7 +2625,7 @@
         <v>407</v>
       </c>
       <c r="G16" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -2648,7 +2648,7 @@
         <v>408</v>
       </c>
       <c r="G17" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -2671,7 +2671,7 @@
         <v>409</v>
       </c>
       <c r="G18" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -2694,7 +2694,7 @@
         <v>410</v>
       </c>
       <c r="G19" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -2717,7 +2717,7 @@
         <v>411</v>
       </c>
       <c r="G20" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -2740,7 +2740,7 @@
         <v>412</v>
       </c>
       <c r="G21" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -2763,7 +2763,7 @@
         <v>413</v>
       </c>
       <c r="G22" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -2786,7 +2786,7 @@
         <v>414</v>
       </c>
       <c r="G23" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2809,7 +2809,7 @@
         <v>415</v>
       </c>
       <c r="G24" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -2832,7 +2832,7 @@
         <v>416</v>
       </c>
       <c r="G25" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -2855,7 +2855,7 @@
         <v>417</v>
       </c>
       <c r="G26" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -2878,7 +2878,7 @@
         <v>418</v>
       </c>
       <c r="G27" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -2901,7 +2901,7 @@
         <v>419</v>
       </c>
       <c r="G28" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -2924,7 +2924,7 @@
         <v>420</v>
       </c>
       <c r="G29" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -2947,7 +2947,7 @@
         <v>421</v>
       </c>
       <c r="G30" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -2970,7 +2970,7 @@
         <v>422</v>
       </c>
       <c r="G31" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2993,7 +2993,7 @@
         <v>423</v>
       </c>
       <c r="G32" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
@@ -3016,7 +3016,7 @@
         <v>424</v>
       </c>
       <c r="G33" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -3039,7 +3039,7 @@
         <v>425</v>
       </c>
       <c r="G34" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -3062,7 +3062,7 @@
         <v>426</v>
       </c>
       <c r="G35" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -3085,7 +3085,7 @@
         <v>427</v>
       </c>
       <c r="G36" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -3108,7 +3108,7 @@
         <v>428</v>
       </c>
       <c r="G37" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
@@ -3131,7 +3131,7 @@
         <v>429</v>
       </c>
       <c r="G38" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -3154,7 +3154,7 @@
         <v>430</v>
       </c>
       <c r="G39" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
@@ -3177,7 +3177,7 @@
         <v>431</v>
       </c>
       <c r="G40" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -3200,7 +3200,7 @@
         <v>432</v>
       </c>
       <c r="G41" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
@@ -3223,7 +3223,7 @@
         <v>433</v>
       </c>
       <c r="G42" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
@@ -3246,7 +3246,7 @@
         <v>434</v>
       </c>
       <c r="G43" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -3269,7 +3269,7 @@
         <v>435</v>
       </c>
       <c r="G44" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -3292,7 +3292,7 @@
         <v>436</v>
       </c>
       <c r="G45" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
@@ -3315,7 +3315,7 @@
         <v>437</v>
       </c>
       <c r="G46" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -3338,7 +3338,7 @@
         <v>438</v>
       </c>
       <c r="G47" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -3361,7 +3361,7 @@
         <v>439</v>
       </c>
       <c r="G48" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
@@ -3384,7 +3384,7 @@
         <v>440</v>
       </c>
       <c r="G49" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -3407,7 +3407,7 @@
         <v>441</v>
       </c>
       <c r="G50" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -3430,7 +3430,7 @@
         <v>442</v>
       </c>
       <c r="G51" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -3453,7 +3453,7 @@
         <v>443</v>
       </c>
       <c r="G52" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
@@ -3476,7 +3476,7 @@
         <v>444</v>
       </c>
       <c r="G53" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
@@ -3499,7 +3499,7 @@
         <v>445</v>
       </c>
       <c r="G54" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
@@ -3522,7 +3522,7 @@
         <v>446</v>
       </c>
       <c r="G55" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
@@ -3545,7 +3545,7 @@
         <v>447</v>
       </c>
       <c r="G56" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
@@ -3568,7 +3568,7 @@
         <v>448</v>
       </c>
       <c r="G57" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
@@ -3591,7 +3591,7 @@
         <v>449</v>
       </c>
       <c r="G58" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
@@ -3614,7 +3614,7 @@
         <v>450</v>
       </c>
       <c r="G59" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
@@ -3637,7 +3637,7 @@
         <v>451</v>
       </c>
       <c r="G60" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
@@ -3660,7 +3660,7 @@
         <v>452</v>
       </c>
       <c r="G61" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
@@ -3683,7 +3683,7 @@
         <v>453</v>
       </c>
       <c r="G62" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
@@ -3706,7 +3706,7 @@
         <v>454</v>
       </c>
       <c r="G63" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
@@ -3729,7 +3729,7 @@
         <v>455</v>
       </c>
       <c r="G64" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
@@ -3752,7 +3752,7 @@
         <v>456</v>
       </c>
       <c r="G65" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
@@ -3775,7 +3775,7 @@
         <v>457</v>
       </c>
       <c r="G66" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
@@ -3789,7 +3789,7 @@
         <v>72</v>
       </c>
       <c r="D67" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="E67" t="s">
         <v>330</v>
@@ -3798,7 +3798,7 @@
         <v>458</v>
       </c>
       <c r="G67" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
@@ -3821,7 +3821,7 @@
         <v>459</v>
       </c>
       <c r="G68" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
@@ -3844,7 +3844,7 @@
         <v>460</v>
       </c>
       <c r="G69" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
@@ -3867,7 +3867,7 @@
         <v>461</v>
       </c>
       <c r="G70" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
@@ -3890,7 +3890,7 @@
         <v>462</v>
       </c>
       <c r="G71" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
@@ -3913,7 +3913,7 @@
         <v>463</v>
       </c>
       <c r="G72" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
@@ -3936,7 +3936,7 @@
         <v>464</v>
       </c>
       <c r="G73" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
@@ -3959,7 +3959,7 @@
         <v>465</v>
       </c>
       <c r="G74" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
@@ -3982,7 +3982,7 @@
         <v>466</v>
       </c>
       <c r="G75" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
@@ -4005,7 +4005,7 @@
         <v>467</v>
       </c>
       <c r="G76" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
@@ -4028,7 +4028,7 @@
         <v>468</v>
       </c>
       <c r="G77" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
@@ -4051,7 +4051,7 @@
         <v>469</v>
       </c>
       <c r="G78" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
@@ -4074,7 +4074,7 @@
         <v>470</v>
       </c>
       <c r="G79" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
@@ -4097,7 +4097,7 @@
         <v>471</v>
       </c>
       <c r="G80" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
@@ -4120,7 +4120,7 @@
         <v>472</v>
       </c>
       <c r="G81" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
@@ -4143,7 +4143,7 @@
         <v>473</v>
       </c>
       <c r="G82" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
@@ -4166,7 +4166,7 @@
         <v>474</v>
       </c>
       <c r="G83" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
@@ -4189,7 +4189,7 @@
         <v>475</v>
       </c>
       <c r="G84" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
@@ -4212,7 +4212,7 @@
         <v>476</v>
       </c>
       <c r="G85" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
@@ -4235,7 +4235,7 @@
         <v>477</v>
       </c>
       <c r="G86" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
@@ -4258,7 +4258,7 @@
         <v>478</v>
       </c>
       <c r="G87" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -4281,7 +4281,7 @@
         <v>479</v>
       </c>
       <c r="G88" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -4304,7 +4304,7 @@
         <v>480</v>
       </c>
       <c r="G89" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -4327,7 +4327,7 @@
         <v>481</v>
       </c>
       <c r="G90" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -4350,7 +4350,7 @@
         <v>482</v>
       </c>
       <c r="G91" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
@@ -4373,7 +4373,7 @@
         <v>483</v>
       </c>
       <c r="G92" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
@@ -4396,7 +4396,7 @@
         <v>484</v>
       </c>
       <c r="G93" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
@@ -4419,7 +4419,7 @@
         <v>485</v>
       </c>
       <c r="G94" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
@@ -4442,7 +4442,7 @@
         <v>486</v>
       </c>
       <c r="G95" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
@@ -4465,7 +4465,7 @@
         <v>487</v>
       </c>
       <c r="G96" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
@@ -4488,7 +4488,7 @@
         <v>488</v>
       </c>
       <c r="G97" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
@@ -4502,7 +4502,7 @@
         <v>103</v>
       </c>
       <c r="D98" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E98" t="s">
         <v>361</v>
@@ -4511,7 +4511,7 @@
         <v>489</v>
       </c>
       <c r="G98" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
@@ -4534,7 +4534,7 @@
         <v>490</v>
       </c>
       <c r="G99" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
@@ -4557,7 +4557,7 @@
         <v>491</v>
       </c>
       <c r="G100" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
@@ -4580,7 +4580,7 @@
         <v>492</v>
       </c>
       <c r="G101" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
@@ -4603,7 +4603,7 @@
         <v>493</v>
       </c>
       <c r="G102" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>494</v>
       </c>
       <c r="G103" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
@@ -4649,7 +4649,7 @@
         <v>495</v>
       </c>
       <c r="G104" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
@@ -4672,7 +4672,7 @@
         <v>496</v>
       </c>
       <c r="G105" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
@@ -4695,7 +4695,7 @@
         <v>497</v>
       </c>
       <c r="G106" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
@@ -4718,7 +4718,7 @@
         <v>498</v>
       </c>
       <c r="G107" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
@@ -4741,7 +4741,7 @@
         <v>499</v>
       </c>
       <c r="G108" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
@@ -4764,7 +4764,7 @@
         <v>500</v>
       </c>
       <c r="G109" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
@@ -4787,7 +4787,7 @@
         <v>501</v>
       </c>
       <c r="G110" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
@@ -4810,7 +4810,7 @@
         <v>502</v>
       </c>
       <c r="G111" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
@@ -4833,7 +4833,7 @@
         <v>503</v>
       </c>
       <c r="G112" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
@@ -4856,7 +4856,7 @@
         <v>504</v>
       </c>
       <c r="G113" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
@@ -4879,7 +4879,7 @@
         <v>505</v>
       </c>
       <c r="G114" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
@@ -4899,10 +4899,10 @@
         <v>377</v>
       </c>
       <c r="F115" t="s">
-        <v>506</v>
+        <v>624</v>
       </c>
       <c r="G115" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
@@ -4922,10 +4922,10 @@
         <v>378</v>
       </c>
       <c r="F116" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="G116" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
@@ -4945,10 +4945,10 @@
         <v>379</v>
       </c>
       <c r="F117" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G117" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
@@ -4968,10 +4968,10 @@
         <v>380</v>
       </c>
       <c r="F118" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G118" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
@@ -4991,10 +4991,10 @@
         <v>381</v>
       </c>
       <c r="F119" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G119" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
@@ -5014,10 +5014,10 @@
         <v>382</v>
       </c>
       <c r="F120" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G120" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
@@ -5037,10 +5037,10 @@
         <v>383</v>
       </c>
       <c r="F121" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G121" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
@@ -5060,10 +5060,10 @@
         <v>384</v>
       </c>
       <c r="F122" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="G122" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
@@ -5083,10 +5083,10 @@
         <v>385</v>
       </c>
       <c r="F123" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="G123" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
@@ -5106,10 +5106,10 @@
         <v>386</v>
       </c>
       <c r="F124" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="G124" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
@@ -5129,10 +5129,10 @@
         <v>386</v>
       </c>
       <c r="F125" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G125" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
@@ -5152,10 +5152,10 @@
         <v>387</v>
       </c>
       <c r="F126" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G126" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
@@ -5175,10 +5175,10 @@
         <v>388</v>
       </c>
       <c r="F127" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G127" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
@@ -5198,10 +5198,10 @@
         <v>389</v>
       </c>
       <c r="F128" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G128" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
@@ -5215,16 +5215,16 @@
         <v>134</v>
       </c>
       <c r="D129" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="E129" t="s">
         <v>390</v>
       </c>
       <c r="F129" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G129" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
@@ -5244,10 +5244,10 @@
         <v>391</v>
       </c>
       <c r="F130" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G130" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -5267,10 +5267,10 @@
         <v>392</v>
       </c>
       <c r="F131" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G131" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -5290,10 +5290,10 @@
         <v>393</v>
       </c>
       <c r="F132" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G132" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
   </sheetData>

</xml_diff>